<commit_message>
Alteração no Caso de uso, diagrama de classe e da user stor.
</commit_message>
<xml_diff>
--- a/Documentação/User Story/UserStory.xlsx
+++ b/Documentação/User Story/UserStory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="20730" windowHeight="9555"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="20730" windowHeight="9555" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Matriz de Dependencia</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -282,7 +285,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +295,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -430,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -509,6 +524,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,9 +864,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,7 +899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>14</v>
       </c>
@@ -887,105 +910,119 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="3">
+        <v>4</v>
+      </c>
+      <c r="D3" s="29"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3">
+        <v>4</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="3">
+        <v>3</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -998,7 +1035,9 @@
       <c r="B11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="3">
+        <v>4</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1011,7 +1050,9 @@
       <c r="B12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="3">
+        <v>4</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1024,7 +1065,9 @@
       <c r="B13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="3">
+        <v>4</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1037,7 +1080,9 @@
       <c r="B14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="3">
+        <v>4</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1050,7 +1095,9 @@
       <c r="B15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="3">
+        <v>4</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1063,7 +1110,9 @@
       <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="3">
+        <v>4</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1076,7 +1125,9 @@
       <c r="B17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="3">
+        <v>4</v>
+      </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1089,7 +1140,9 @@
       <c r="B18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="3">
+        <v>4</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -1102,7 +1155,9 @@
       <c r="B19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1115,7 +1170,9 @@
       <c r="B20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="3">
+        <v>4</v>
+      </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1128,7 +1185,9 @@
       <c r="B21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="3">
+        <v>3</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1141,7 +1200,9 @@
       <c r="B22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1154,7 +1215,9 @@
       <c r="B23" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -1167,7 +1230,9 @@
       <c r="B24" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -1180,7 +1245,9 @@
       <c r="B25" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="3">
+        <v>1</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1231,7 +1298,7 @@
       <c r="B30" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1244,7 +1311,7 @@
       <c r="B31" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1257,7 +1324,7 @@
       <c r="B32" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="3"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -1281,7 +1348,7 @@
       <c r="B34" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="4"/>
+      <c r="C34" s="3"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1294,7 +1361,7 @@
       <c r="B35" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="3"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1307,7 +1374,7 @@
       <c r="B36" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="4"/>
+      <c r="C36" s="3"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -1320,7 +1387,7 @@
       <c r="B37" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="4"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1353,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF33"/>
+  <dimension ref="A1:AG33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1431,7 @@
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:33" ht="21" x14ac:dyDescent="0.35">
       <c r="C1" s="19" t="s">
         <v>45</v>
       </c>
@@ -1374,7 +1441,7 @@
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C2" s="13">
         <v>1</v>
       </c>
@@ -1465,1184 +1532,1260 @@
       <c r="AF2" s="13">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="AG2" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4"/>
-      <c r="AF3" s="4"/>
-    </row>
-    <row r="4" spans="1:32" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="C3" s="30"/>
+      <c r="D3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="4"/>
+    </row>
+    <row r="4" spans="1:33" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-    </row>
-    <row r="5" spans="1:32" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="C4" s="3"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="4"/>
+    </row>
+    <row r="5" spans="1:33" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
-    </row>
-    <row r="6" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="30"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="4"/>
+    </row>
+    <row r="6" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="4"/>
-      <c r="AF6" s="4"/>
-    </row>
-    <row r="7" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="4"/>
+    </row>
+    <row r="7" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="4"/>
-      <c r="AB7" s="4"/>
-      <c r="AC7" s="4"/>
-      <c r="AD7" s="4"/>
-      <c r="AE7" s="4"/>
-      <c r="AF7" s="4"/>
-    </row>
-    <row r="8" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="4"/>
+    </row>
+    <row r="8" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-      <c r="AA8" s="4"/>
-      <c r="AB8" s="4"/>
-      <c r="AC8" s="4"/>
-      <c r="AD8" s="4"/>
-      <c r="AE8" s="4"/>
-      <c r="AF8" s="4"/>
-    </row>
-    <row r="9" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="4"/>
+    </row>
+    <row r="9" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="4"/>
-      <c r="AB9" s="4"/>
-      <c r="AC9" s="4"/>
-      <c r="AD9" s="4"/>
-      <c r="AE9" s="4"/>
-      <c r="AF9" s="4"/>
-    </row>
-    <row r="10" spans="1:32" ht="72" x14ac:dyDescent="0.3">
+      <c r="C9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="4"/>
+    </row>
+    <row r="10" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="4"/>
-      <c r="AB10" s="4"/>
-      <c r="AC10" s="4"/>
-      <c r="AD10" s="4"/>
-      <c r="AE10" s="4"/>
-      <c r="AF10" s="4"/>
-    </row>
-    <row r="11" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="4"/>
+    </row>
+    <row r="11" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
-      <c r="AA11" s="4"/>
-      <c r="AB11" s="4"/>
-      <c r="AC11" s="4"/>
-      <c r="AD11" s="4"/>
-      <c r="AE11" s="4"/>
-      <c r="AF11" s="4"/>
-    </row>
-    <row r="12" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="4"/>
+    </row>
+    <row r="12" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="4"/>
-      <c r="AC12" s="4"/>
-      <c r="AD12" s="4"/>
-      <c r="AE12" s="4"/>
-      <c r="AF12" s="4"/>
-    </row>
-    <row r="13" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="4"/>
+    </row>
+    <row r="13" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
-      <c r="AB13" s="4"/>
-      <c r="AC13" s="4"/>
-      <c r="AD13" s="4"/>
-      <c r="AE13" s="4"/>
-      <c r="AF13" s="4"/>
-    </row>
-    <row r="14" spans="1:32" ht="75" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="4"/>
+    </row>
+    <row r="14" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="4"/>
-      <c r="AC14" s="4"/>
-      <c r="AD14" s="4"/>
-      <c r="AE14" s="4"/>
-      <c r="AF14" s="4"/>
-    </row>
-    <row r="15" spans="1:32" ht="75" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="4"/>
+    </row>
+    <row r="15" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="4"/>
-      <c r="AD15" s="4"/>
-      <c r="AE15" s="4"/>
-      <c r="AF15" s="4"/>
-    </row>
-    <row r="16" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="4"/>
+    </row>
+    <row r="16" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
-      <c r="AB16" s="4"/>
-      <c r="AC16" s="4"/>
-      <c r="AD16" s="4"/>
-      <c r="AE16" s="4"/>
-      <c r="AF16" s="4"/>
-    </row>
-    <row r="17" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="4"/>
+    </row>
+    <row r="17" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
-      <c r="AB17" s="4"/>
-      <c r="AC17" s="4"/>
-      <c r="AD17" s="4"/>
-      <c r="AE17" s="4"/>
-      <c r="AF17" s="4"/>
-    </row>
-    <row r="18" spans="1:32" ht="75" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="4"/>
+    </row>
+    <row r="18" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="4"/>
-      <c r="AB18" s="4"/>
-      <c r="AC18" s="4"/>
-      <c r="AD18" s="4"/>
-      <c r="AE18" s="4"/>
-      <c r="AF18" s="4"/>
-    </row>
-    <row r="19" spans="1:32" ht="75" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="4"/>
+    </row>
+    <row r="19" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
-      <c r="AA19" s="4"/>
-      <c r="AB19" s="4"/>
-      <c r="AC19" s="4"/>
-      <c r="AD19" s="4"/>
-      <c r="AE19" s="4"/>
-      <c r="AF19" s="4"/>
-    </row>
-    <row r="20" spans="1:32" ht="75" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="3"/>
+      <c r="AG19" s="4"/>
+    </row>
+    <row r="20" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="4"/>
-      <c r="AB20" s="4"/>
-      <c r="AC20" s="4"/>
-      <c r="AD20" s="4"/>
-      <c r="AE20" s="4"/>
-      <c r="AF20" s="4"/>
-    </row>
-    <row r="21" spans="1:32" ht="90" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="4"/>
+    </row>
+    <row r="21" spans="1:33" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
-      <c r="AB21" s="4"/>
-      <c r="AC21" s="4"/>
-      <c r="AD21" s="4"/>
-      <c r="AE21" s="4"/>
-      <c r="AF21" s="4"/>
-    </row>
-    <row r="22" spans="1:32" ht="90" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="30"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="3"/>
+      <c r="AG21" s="4"/>
+    </row>
+    <row r="22" spans="1:33" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="4"/>
-      <c r="AB22" s="4"/>
-      <c r="AC22" s="4"/>
-      <c r="AD22" s="4"/>
-      <c r="AE22" s="4"/>
-      <c r="AF22" s="4"/>
-    </row>
-    <row r="23" spans="1:32" ht="75" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="30"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="4"/>
+    </row>
+    <row r="23" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
-      <c r="Z23" s="4"/>
-      <c r="AA23" s="4"/>
-      <c r="AB23" s="4"/>
-      <c r="AC23" s="4"/>
-      <c r="AD23" s="4"/>
-      <c r="AE23" s="4"/>
-      <c r="AF23" s="4"/>
-    </row>
-    <row r="24" spans="1:32" ht="90" x14ac:dyDescent="0.25">
+      <c r="C23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="4"/>
+    </row>
+    <row r="24" spans="1:33" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
-      <c r="Z24" s="4"/>
-      <c r="AA24" s="4"/>
-      <c r="AB24" s="4"/>
-      <c r="AC24" s="4"/>
-      <c r="AD24" s="4"/>
-      <c r="AE24" s="4"/>
-      <c r="AF24" s="4"/>
-    </row>
-    <row r="25" spans="1:32" ht="105" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="4"/>
+    </row>
+    <row r="25" spans="1:33" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
-      <c r="AA25" s="4"/>
-      <c r="AB25" s="4"/>
-      <c r="AC25" s="4"/>
-      <c r="AD25" s="4"/>
-      <c r="AE25" s="4"/>
-      <c r="AF25" s="4"/>
-    </row>
-    <row r="26" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+      <c r="C25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="30"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="4"/>
+    </row>
+    <row r="26" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
-      <c r="AA26" s="4"/>
-      <c r="AB26" s="4"/>
-      <c r="AC26" s="4"/>
-      <c r="AD26" s="4"/>
-      <c r="AE26" s="4"/>
-      <c r="AF26" s="4"/>
-    </row>
-    <row r="27" spans="1:32" ht="45" x14ac:dyDescent="0.25">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="30"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="4"/>
+    </row>
+    <row r="27" spans="1:33" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
-      <c r="AA27" s="4"/>
-      <c r="AB27" s="4"/>
-      <c r="AC27" s="4"/>
-      <c r="AD27" s="4"/>
-      <c r="AE27" s="4"/>
-      <c r="AF27" s="4"/>
-    </row>
-    <row r="28" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="30"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="4"/>
+    </row>
+    <row r="28" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
-      <c r="AA28" s="4"/>
-      <c r="AB28" s="4"/>
-      <c r="AC28" s="4"/>
-      <c r="AD28" s="4"/>
-      <c r="AE28" s="4"/>
-      <c r="AF28" s="4"/>
-    </row>
-    <row r="29" spans="1:32" ht="75" x14ac:dyDescent="0.25">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="30"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="4"/>
+    </row>
+    <row r="29" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
-      <c r="AA29" s="4"/>
-      <c r="AB29" s="4"/>
-      <c r="AC29" s="4"/>
-      <c r="AD29" s="4"/>
-      <c r="AE29" s="4"/>
-      <c r="AF29" s="4"/>
-    </row>
-    <row r="30" spans="1:32" ht="75" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="30"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="3"/>
+      <c r="AG29" s="4"/>
+    </row>
+    <row r="30" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
-      <c r="Z30" s="4"/>
-      <c r="AA30" s="4"/>
-      <c r="AB30" s="4"/>
-      <c r="AC30" s="4"/>
-      <c r="AD30" s="4"/>
-      <c r="AE30" s="4"/>
-      <c r="AF30" s="4"/>
-    </row>
-    <row r="31" spans="1:32" ht="75" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="30"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="4"/>
+    </row>
+    <row r="31" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
-      <c r="Z31" s="4"/>
-      <c r="AA31" s="4"/>
-      <c r="AB31" s="4"/>
-      <c r="AC31" s="4"/>
-      <c r="AD31" s="4"/>
-      <c r="AE31" s="4"/>
-      <c r="AF31" s="4"/>
-    </row>
-    <row r="32" spans="1:32" ht="75" x14ac:dyDescent="0.25">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="3"/>
+      <c r="AE31" s="30"/>
+      <c r="AF31" s="3"/>
+      <c r="AG31" s="4"/>
+    </row>
+    <row r="32" spans="1:33" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
-      <c r="AA32" s="4"/>
-      <c r="AB32" s="4"/>
-      <c r="AC32" s="4"/>
-      <c r="AD32" s="4"/>
-      <c r="AE32" s="4"/>
-      <c r="AF32" s="4"/>
-    </row>
-    <row r="33" spans="1:32" ht="105" x14ac:dyDescent="0.25">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="3"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="30"/>
+      <c r="AG32" s="4"/>
+    </row>
+    <row r="33" spans="1:33" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
-      <c r="AA33" s="4"/>
-      <c r="AB33" s="4"/>
-      <c r="AC33" s="4"/>
-      <c r="AD33" s="4"/>
-      <c r="AE33" s="4"/>
-      <c r="AF33" s="4"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="3"/>
+      <c r="AG33" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Adição das users stores de Listar.
</commit_message>
<xml_diff>
--- a/Documentação/User Story/UserStory.xlsx
+++ b/Documentação/User Story/UserStory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="11616" windowHeight="9684"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="11610" windowHeight="9690"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -240,6 +240,36 @@
   <si>
     <t>Como Desenvolvedor
 Quero configurar meu ambiente de trabalho</t>
+  </si>
+  <si>
+    <t>Como Personal
+Quero listar as Avaliações Físicas de um aluno
+Para que possa visualizalas</t>
+  </si>
+  <si>
+    <t>Como Personal
+Quero listar as Sereies de um aluno
+Para que possa visualizalas</t>
+  </si>
+  <si>
+    <t>Como Personal
+Quero listar os Alunos
+Para que possa visualizalos</t>
+  </si>
+  <si>
+    <t>Como Personal
+Quero listar os Exercícios
+Para que possa Selecionalos</t>
+  </si>
+  <si>
+    <t>Como Aluno
+Quero listar as Minhas Séries
+Para que possa Visualizalas</t>
+  </si>
+  <si>
+    <t>Como Aluno
+Quero listar as minhas Avaliações Físicas 
+Para que possa visualizalas</t>
   </si>
 </sst>
 </file>
@@ -2180,7 +2210,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2218,7 +2248,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2290,7 +2320,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2468,7 +2498,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -2477,24 +2507,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
-    </sheetView>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="4.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="48.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="77" t="s">
         <v>0</v>
       </c>
@@ -2515,7 +2543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="78"/>
       <c r="C3" s="80"/>
       <c r="D3" s="13" t="s">
@@ -2539,7 +2567,7 @@
       <c r="G4" s="67"/>
       <c r="H4" s="68"/>
     </row>
-    <row r="5" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="46.9" x14ac:dyDescent="0.3">
       <c r="B5" s="14">
         <v>1</v>
       </c>
@@ -2560,7 +2588,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="46.9" x14ac:dyDescent="0.3">
       <c r="B6" s="15">
         <v>2</v>
       </c>
@@ -2581,7 +2609,7 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="46.9" x14ac:dyDescent="0.3">
       <c r="B7" s="15">
         <v>3</v>
       </c>
@@ -2602,7 +2630,7 @@
       </c>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="46.9" x14ac:dyDescent="0.3">
       <c r="B8" s="15">
         <v>4</v>
       </c>
@@ -2623,7 +2651,7 @@
       </c>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="46.9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -2647,7 +2675,7 @@
       </c>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="46.9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2671,7 +2699,7 @@
       </c>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="46.9" x14ac:dyDescent="0.3">
       <c r="B11" s="15">
         <v>7</v>
       </c>
@@ -2692,7 +2720,7 @@
       </c>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="46.9" x14ac:dyDescent="0.3">
       <c r="B12" s="15">
         <v>8</v>
       </c>
@@ -2713,7 +2741,7 @@
       </c>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B13" s="15">
         <v>9</v>
       </c>
@@ -2734,7 +2762,7 @@
       </c>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B14" s="15">
         <v>10</v>
       </c>
@@ -2755,7 +2783,7 @@
       </c>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B15" s="15">
         <v>11</v>
       </c>
@@ -2776,7 +2804,7 @@
       </c>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B16" s="15">
         <v>12</v>
       </c>
@@ -2797,7 +2825,7 @@
       </c>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B17" s="15">
         <v>13</v>
       </c>
@@ -2818,7 +2846,7 @@
       </c>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B18" s="15">
         <v>14</v>
       </c>
@@ -2839,7 +2867,7 @@
       </c>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B19" s="15">
         <v>15</v>
       </c>
@@ -2860,7 +2888,7 @@
       </c>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B20" s="15">
         <v>16</v>
       </c>
@@ -2881,7 +2909,7 @@
       </c>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B21" s="15">
         <v>17</v>
       </c>
@@ -2902,7 +2930,7 @@
       </c>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B22" s="15">
         <v>18</v>
       </c>
@@ -2923,7 +2951,7 @@
       </c>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="2:8" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="63" x14ac:dyDescent="0.25">
       <c r="B23" s="15">
         <v>19</v>
       </c>
@@ -2944,7 +2972,7 @@
       </c>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="2:8" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="63" x14ac:dyDescent="0.25">
       <c r="B24" s="15">
         <v>20</v>
       </c>
@@ -2965,7 +2993,7 @@
       </c>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B25" s="15">
         <v>21</v>
       </c>
@@ -2986,7 +3014,7 @@
       </c>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B26" s="15">
         <v>22</v>
       </c>
@@ -3007,7 +3035,7 @@
       </c>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="2:8" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="16">
         <v>23</v>
       </c>
@@ -3028,7 +3056,7 @@
       </c>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="66" t="s">
         <v>12</v>
       </c>
@@ -3039,7 +3067,7 @@
       <c r="G28" s="67"/>
       <c r="H28" s="68"/>
     </row>
-    <row r="29" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B29" s="14">
         <v>24</v>
       </c>
@@ -3060,7 +3088,7 @@
       </c>
       <c r="H29" s="9"/>
     </row>
-    <row r="30" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B30" s="15">
         <v>25</v>
       </c>
@@ -3081,7 +3109,7 @@
       </c>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" spans="2:8" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="16">
         <v>26</v>
       </c>
@@ -3102,7 +3130,7 @@
       </c>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" spans="2:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="16">
         <v>27</v>
       </c>
@@ -3123,7 +3151,7 @@
       </c>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="66" t="s">
         <v>13</v>
       </c>
@@ -3134,7 +3162,7 @@
       <c r="G33" s="67"/>
       <c r="H33" s="68"/>
     </row>
-    <row r="34" spans="2:8" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="16">
         <v>28</v>
       </c>
@@ -3155,8 +3183,146 @@
       </c>
       <c r="H34" s="11"/>
     </row>
+    <row r="35" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="67"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="67"/>
+      <c r="H35" s="68"/>
+    </row>
+    <row r="36" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="16">
+        <v>29</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="52">
+        <v>4</v>
+      </c>
+      <c r="E36" s="58">
+        <v>3</v>
+      </c>
+      <c r="F36" s="58">
+        <v>3</v>
+      </c>
+      <c r="G36" s="63">
+        <v>3</v>
+      </c>
+      <c r="H36" s="11"/>
+    </row>
+    <row r="37" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="16">
+        <v>30</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="52">
+        <v>4</v>
+      </c>
+      <c r="E37" s="58">
+        <v>3</v>
+      </c>
+      <c r="F37" s="58">
+        <v>3</v>
+      </c>
+      <c r="G37" s="63">
+        <v>3</v>
+      </c>
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="16">
+        <v>31</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="52">
+        <v>4</v>
+      </c>
+      <c r="E38" s="58">
+        <v>3</v>
+      </c>
+      <c r="F38" s="58">
+        <v>3</v>
+      </c>
+      <c r="G38" s="63">
+        <v>3</v>
+      </c>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="16">
+        <v>32</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="52">
+        <v>4</v>
+      </c>
+      <c r="E39" s="58">
+        <v>3</v>
+      </c>
+      <c r="F39" s="58">
+        <v>3</v>
+      </c>
+      <c r="G39" s="63">
+        <v>3</v>
+      </c>
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="16">
+        <v>33</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="52">
+        <v>4</v>
+      </c>
+      <c r="E40" s="58">
+        <v>3</v>
+      </c>
+      <c r="F40" s="58">
+        <v>3</v>
+      </c>
+      <c r="G40" s="63">
+        <v>3</v>
+      </c>
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="2:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="16">
+        <v>34</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="52">
+        <v>4</v>
+      </c>
+      <c r="E41" s="58">
+        <v>3</v>
+      </c>
+      <c r="F41" s="58">
+        <v>3</v>
+      </c>
+      <c r="G41" s="63">
+        <v>3</v>
+      </c>
+      <c r="H41" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="B35:H35"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B28:H28"/>
     <mergeCell ref="B33:H33"/>
@@ -3181,16 +3347,16 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="42.5546875" style="22" customWidth="1"/>
-    <col min="4" max="34" width="4.6640625" style="22" customWidth="1"/>
-    <col min="35" max="16384" width="9.109375" style="22"/>
+    <col min="1" max="1" width="3.42578125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="22" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" style="22" customWidth="1"/>
+    <col min="4" max="34" width="4.7109375" style="22" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:34" ht="14.45" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:34" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="23"/>
       <c r="C2" s="24"/>
@@ -3228,7 +3394,7 @@
       <c r="AG2" s="81"/>
       <c r="AH2" s="82"/>
     </row>
-    <row r="3" spans="2:34" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:34" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="25"/>
       <c r="C3" s="26"/>
       <c r="D3" s="27">
@@ -3325,7 +3491,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:34" ht="46.95" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:34" ht="46.9" x14ac:dyDescent="0.4">
       <c r="B4" s="29">
         <v>1</v>
       </c>
@@ -3364,7 +3530,7 @@
       <c r="AG4" s="42"/>
       <c r="AH4" s="43"/>
     </row>
-    <row r="5" spans="2:34" ht="46.95" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:34" ht="46.9" x14ac:dyDescent="0.4">
       <c r="B5" s="15">
         <v>2</v>
       </c>
@@ -3405,7 +3571,7 @@
       <c r="AG5" s="46"/>
       <c r="AH5" s="47"/>
     </row>
-    <row r="6" spans="2:34" ht="46.95" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:34" ht="46.9" x14ac:dyDescent="0.4">
       <c r="B6" s="15">
         <v>3</v>
       </c>
@@ -3448,7 +3614,7 @@
       <c r="AG6" s="46"/>
       <c r="AH6" s="47"/>
     </row>
-    <row r="7" spans="2:34" ht="46.95" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:34" ht="46.9" x14ac:dyDescent="0.4">
       <c r="B7" s="15">
         <v>4</v>
       </c>
@@ -3491,7 +3657,7 @@
       <c r="AG7" s="46"/>
       <c r="AH7" s="47"/>
     </row>
-    <row r="8" spans="2:34" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:34" ht="46.9" x14ac:dyDescent="0.4">
       <c r="B8" s="15">
         <v>5</v>
       </c>
@@ -3536,7 +3702,7 @@
       <c r="AG8" s="46"/>
       <c r="AH8" s="47"/>
     </row>
-    <row r="9" spans="2:34" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:34" ht="46.9" x14ac:dyDescent="0.4">
       <c r="B9" s="15">
         <v>6</v>
       </c>
@@ -3583,7 +3749,7 @@
       <c r="AG9" s="46"/>
       <c r="AH9" s="47"/>
     </row>
-    <row r="10" spans="2:34" ht="46.95" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:34" ht="46.9" x14ac:dyDescent="0.4">
       <c r="B10" s="15">
         <v>7</v>
       </c>
@@ -3628,7 +3794,7 @@
       <c r="AG10" s="46"/>
       <c r="AH10" s="47"/>
     </row>
-    <row r="11" spans="2:34" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:34" ht="46.9" x14ac:dyDescent="0.4">
       <c r="B11" s="15">
         <v>8</v>
       </c>
@@ -3675,7 +3841,7 @@
       <c r="AG11" s="46"/>
       <c r="AH11" s="47"/>
     </row>
-    <row r="12" spans="2:34" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:34" ht="47.25" x14ac:dyDescent="0.35">
       <c r="B12" s="15">
         <v>9</v>
       </c>
@@ -3718,7 +3884,7 @@
       <c r="AG12" s="46"/>
       <c r="AH12" s="47"/>
     </row>
-    <row r="13" spans="2:34" ht="62.4" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:34" ht="47.25" x14ac:dyDescent="0.35">
       <c r="B13" s="15">
         <v>10</v>
       </c>
@@ -3763,7 +3929,7 @@
       <c r="AG13" s="46"/>
       <c r="AH13" s="47"/>
     </row>
-    <row r="14" spans="2:34" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:34" ht="47.25" x14ac:dyDescent="0.35">
       <c r="B14" s="15">
         <v>11</v>
       </c>
@@ -3808,7 +3974,7 @@
       <c r="AG14" s="46"/>
       <c r="AH14" s="47"/>
     </row>
-    <row r="15" spans="2:34" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:34" ht="47.25" x14ac:dyDescent="0.35">
       <c r="B15" s="15">
         <v>12</v>
       </c>
@@ -3855,7 +4021,7 @@
       <c r="AG15" s="46"/>
       <c r="AH15" s="47"/>
     </row>
-    <row r="16" spans="2:34" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:34" ht="47.25" x14ac:dyDescent="0.35">
       <c r="B16" s="15">
         <v>13</v>
       </c>
@@ -3904,7 +4070,7 @@
       <c r="AG16" s="46"/>
       <c r="AH16" s="47"/>
     </row>
-    <row r="17" spans="2:34" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:34" ht="47.25" x14ac:dyDescent="0.35">
       <c r="B17" s="15">
         <v>14</v>
       </c>
@@ -3953,7 +4119,7 @@
       <c r="AG17" s="46"/>
       <c r="AH17" s="47"/>
     </row>
-    <row r="18" spans="2:34" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:34" ht="47.25" x14ac:dyDescent="0.35">
       <c r="B18" s="15">
         <v>15</v>
       </c>
@@ -3998,7 +4164,7 @@
       <c r="AG18" s="46"/>
       <c r="AH18" s="47"/>
     </row>
-    <row r="19" spans="2:34" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:34" ht="47.25" x14ac:dyDescent="0.35">
       <c r="B19" s="15">
         <v>16</v>
       </c>
@@ -4045,7 +4211,7 @@
       <c r="AG19" s="46"/>
       <c r="AH19" s="47"/>
     </row>
-    <row r="20" spans="2:34" ht="62.4" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:34" ht="63" x14ac:dyDescent="0.35">
       <c r="B20" s="15">
         <v>17</v>
       </c>
@@ -4094,7 +4260,7 @@
       <c r="AG20" s="46"/>
       <c r="AH20" s="47"/>
     </row>
-    <row r="21" spans="2:34" ht="62.4" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:34" ht="47.25" x14ac:dyDescent="0.35">
       <c r="B21" s="15">
         <v>18</v>
       </c>
@@ -4141,7 +4307,7 @@
       <c r="AG21" s="46"/>
       <c r="AH21" s="47"/>
     </row>
-    <row r="22" spans="2:34" ht="62.4" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:34" ht="63" x14ac:dyDescent="0.35">
       <c r="B22" s="15">
         <v>19</v>
       </c>
@@ -4188,7 +4354,7 @@
       <c r="AG22" s="46"/>
       <c r="AH22" s="47"/>
     </row>
-    <row r="23" spans="2:34" ht="62.4" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:34" ht="63" x14ac:dyDescent="0.35">
       <c r="B23" s="15">
         <v>20</v>
       </c>
@@ -4233,7 +4399,7 @@
       <c r="AG23" s="46"/>
       <c r="AH23" s="47"/>
     </row>
-    <row r="24" spans="2:34" ht="62.4" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:34" ht="63" x14ac:dyDescent="0.35">
       <c r="B24" s="15">
         <v>21</v>
       </c>
@@ -4284,7 +4450,7 @@
       <c r="AG24" s="46"/>
       <c r="AH24" s="47"/>
     </row>
-    <row r="25" spans="2:34" ht="78" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:34" ht="78.75" x14ac:dyDescent="0.35">
       <c r="B25" s="15">
         <v>22</v>
       </c>
@@ -4333,7 +4499,7 @@
       <c r="AG25" s="46"/>
       <c r="AH25" s="47"/>
     </row>
-    <row r="26" spans="2:34" ht="78" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:34" ht="78.75" x14ac:dyDescent="0.35">
       <c r="B26" s="15">
         <v>23</v>
       </c>
@@ -4378,7 +4544,7 @@
       <c r="AG26" s="46"/>
       <c r="AH26" s="47"/>
     </row>
-    <row r="27" spans="2:34" ht="62.4" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:34" ht="47.25" x14ac:dyDescent="0.35">
       <c r="B27" s="15">
         <v>24</v>
       </c>
@@ -4419,7 +4585,7 @@
       <c r="AG27" s="46"/>
       <c r="AH27" s="47"/>
     </row>
-    <row r="28" spans="2:34" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:34" ht="47.25" x14ac:dyDescent="0.35">
       <c r="B28" s="15">
         <v>25</v>
       </c>
@@ -4462,7 +4628,7 @@
       <c r="AG28" s="46"/>
       <c r="AH28" s="47"/>
     </row>
-    <row r="29" spans="2:34" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:34" ht="47.25" x14ac:dyDescent="0.35">
       <c r="B29" s="15">
         <v>26</v>
       </c>
@@ -4505,7 +4671,7 @@
       <c r="AG29" s="46"/>
       <c r="AH29" s="47"/>
     </row>
-    <row r="30" spans="2:34" ht="31.2" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:34" ht="31.5" x14ac:dyDescent="0.35">
       <c r="B30" s="15">
         <v>27</v>
       </c>
@@ -4544,7 +4710,7 @@
       <c r="AG30" s="46"/>
       <c r="AH30" s="47"/>
     </row>
-    <row r="31" spans="2:34" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:34" ht="79.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="16">
         <v>31</v>
       </c>
@@ -4601,25 +4767,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="29.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" style="6" customWidth="1"/>
     <col min="2" max="2" width="3" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" style="33" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="29.6640625" style="4"/>
+    <col min="3" max="3" width="31.7109375" style="33" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="29.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" s="6" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C1" s="33"/>
     </row>
-    <row r="2" spans="2:7" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="84" t="s">
         <v>33</v>
       </c>
@@ -4629,7 +4793,7 @@
       <c r="F2" s="86"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="89"/>
       <c r="C3" s="90"/>
       <c r="D3" s="83" t="s">
@@ -4640,7 +4804,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="91"/>
       <c r="C4" s="92"/>
       <c r="D4" s="40" t="s">
@@ -4671,7 +4835,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="43.15" x14ac:dyDescent="0.3">
       <c r="B6" s="38">
         <v>2</v>
       </c>
@@ -4691,7 +4855,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="43.15" x14ac:dyDescent="0.3">
       <c r="B7" s="38">
         <v>3</v>
       </c>
@@ -4805,7 +4969,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="38">
         <v>9</v>
       </c>
@@ -4825,7 +4989,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="38">
         <v>10</v>
       </c>
@@ -4845,7 +5009,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="38">
         <v>11</v>
       </c>
@@ -4865,7 +5029,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B16" s="38">
         <v>12</v>
       </c>
@@ -4882,7 +5046,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" s="38">
         <v>13</v>
       </c>
@@ -4899,7 +5063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="38">
         <v>14</v>
       </c>
@@ -4916,7 +5080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <v>15</v>
       </c>
@@ -4933,7 +5097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="38">
         <v>16</v>
       </c>
@@ -4950,7 +5114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B21" s="38">
         <v>17</v>
       </c>
@@ -4967,7 +5131,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B22" s="38">
         <v>18</v>
       </c>
@@ -4984,7 +5148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B23" s="38">
         <v>19</v>
       </c>
@@ -5001,7 +5165,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B24" s="38">
         <v>20</v>
       </c>
@@ -5018,7 +5182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B25" s="38">
         <v>21</v>
       </c>
@@ -5035,7 +5199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B26" s="38">
         <v>22</v>
       </c>
@@ -5052,7 +5216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B27" s="38">
         <v>23</v>
       </c>
@@ -5069,7 +5233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B28" s="38">
         <v>24</v>
       </c>
@@ -5089,7 +5253,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B29" s="38">
         <v>25</v>
       </c>
@@ -5109,7 +5273,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B30" s="38">
         <v>26</v>
       </c>
@@ -5129,7 +5293,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" ht="43.15" x14ac:dyDescent="0.3">
       <c r="B31" s="38">
         <v>27</v>
       </c>
@@ -5146,7 +5310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="39">
         <v>31</v>
       </c>

</xml_diff>